<commit_message>
Images opening functionality was removed. The default amount of files decreased to 75.
</commit_message>
<xml_diff>
--- a/Automation Anywhere/Bots/ADT/Proofs/Ultimate Excel Dashboard.xlsx
+++ b/Automation Anywhere/Bots/ADT/Proofs/Ultimate Excel Dashboard.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\InterfacePerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="759"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="759" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CPU_Data" sheetId="22" r:id="rId1"/>
@@ -1735,10 +1735,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>CPU_Data!$B$2:$B$201</c:f>
+              <c:f>CPU_Data!$B$2:$B$151</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="200"/>
+                <c:ptCount val="150"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1842,6 +1842,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2088,6 +2089,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3071,7 +3073,7 @@
         <c:axId val="641171544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200"/>
+          <c:max val="150"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3131,6 +3133,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7930,7 +7933,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId2"/>
+              <asvg:svgBlip xmlns="" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -7983,7 +7986,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId4"/>
+              <asvg:svgBlip xmlns="" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -8036,7 +8039,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId6"/>
+              <asvg:svgBlip xmlns="" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -8089,7 +8092,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId8"/>
+              <asvg:svgBlip xmlns="" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -10167,7 +10170,7 @@
   </sheetPr>
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -12293,8 +12296,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel Dashboard opening issue fixed.
</commit_message>
<xml_diff>
--- a/Automation Anywhere/Bots/ADT/Proofs/Ultimate Excel Dashboard.xlsx
+++ b/Automation Anywhere/Bots/ADT/Proofs/Ultimate Excel Dashboard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\InterfacePerformance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -10804,9 +10804,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10834,7 +10832,7 @@
   </sheetPr>
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -11468,9 +11466,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12135,9 +12131,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12297,7 +12291,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>